<commit_message>
Updated BIC codes for DE, AT and NL & updated source for NL
</commit_message>
<xml_diff>
--- a/data/nl.xlsx
+++ b/data/nl.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\asp.local\CR-home$\k.meijer_cr\Windows\Profile.v4\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="19020" windowHeight="10875"/>
   </bookViews>
@@ -14,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="201">
-  <si>
-    <t>CITIBANK INTERNATIONAL PLC</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="205">
   <si>
     <t>LOMBARD ODIER DARIER HENTSCH &amp; CIE</t>
   </si>
@@ -133,18 +135,12 @@
     <t>RABONL2U</t>
   </si>
   <si>
-    <t>RBOSNL2A</t>
-  </si>
-  <si>
     <t>SNSBNL2A</t>
   </si>
   <si>
     <t>SOGENL2A</t>
   </si>
   <si>
-    <t>STALNL2G</t>
-  </si>
-  <si>
     <t>TEBUNL2A</t>
   </si>
   <si>
@@ -274,18 +270,12 @@
     <t>RABO</t>
   </si>
   <si>
-    <t>RBOS</t>
-  </si>
-  <si>
     <t>SNSB</t>
   </si>
   <si>
     <t>SOGE</t>
   </si>
   <si>
-    <t>STAL</t>
-  </si>
-  <si>
     <t>TEBU</t>
   </si>
   <si>
@@ -349,9 +339,6 @@
     <t>REGIOBANK</t>
   </si>
   <si>
-    <t>(SVENSKA) HANDELSBANKEN AB</t>
-  </si>
-  <si>
     <t>ICBK</t>
   </si>
   <si>
@@ -373,9 +360,6 @@
     <t>FRGH</t>
   </si>
   <si>
-    <t>FRIESCH GRONINGSE HYPOTHEEK BANK</t>
-  </si>
-  <si>
     <t>FRGHNL21</t>
   </si>
   <si>
@@ -391,9 +375,6 @@
     <t>ZWLBNL21</t>
   </si>
   <si>
-    <t>ZWITSERLEVENBANK</t>
-  </si>
-  <si>
     <t>BLGW</t>
   </si>
   <si>
@@ -409,9 +390,6 @@
     <t>ASN BANK</t>
   </si>
   <si>
-    <t>INDUSTRIAL AND COMMERCIAL BANK OF CHINA</t>
-  </si>
-  <si>
     <t>CHAS</t>
   </si>
   <si>
@@ -424,211 +402,257 @@
     <t>ANAA</t>
   </si>
   <si>
+    <t>BKCH</t>
+  </si>
+  <si>
+    <t>BANK OF CHINA</t>
+  </si>
+  <si>
+    <t>BKCHNL2R</t>
+  </si>
+  <si>
+    <t>BMEU</t>
+  </si>
+  <si>
+    <t>BMEUNL21</t>
+  </si>
+  <si>
+    <t>BMCE EUROSERVICES</t>
+  </si>
+  <si>
+    <t>BINKNL21</t>
+  </si>
+  <si>
+    <t>BINK</t>
+  </si>
+  <si>
+    <t>BUNQ</t>
+  </si>
+  <si>
+    <t>BUNQNL2A</t>
+  </si>
+  <si>
+    <t>PCBC</t>
+  </si>
+  <si>
+    <t>PCBCNL2A</t>
+  </si>
+  <si>
+    <t>BANQUE CHAABI DU MAROC</t>
+  </si>
+  <si>
+    <t>ISBANK</t>
+  </si>
+  <si>
+    <t>KOREA EXCHANGE BANK</t>
+  </si>
+  <si>
+    <t>SOCIETE GENERALE</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN BANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABN AMRO BANK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AEGON BANK </t>
+  </si>
+  <si>
+    <t>ANADOLUBANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACHMEA BANK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARGENTA SPAARBANK </t>
+  </si>
+  <si>
+    <t>AMSTERDAM TRADE BANK</t>
+  </si>
+  <si>
+    <t>INTESA SANPAOLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BINCKBANK </t>
+  </si>
+  <si>
+    <t>BINCKBANK, PROF</t>
+  </si>
+  <si>
+    <t>BANK MENDES GANS</t>
+  </si>
+  <si>
+    <t>BANK NEDERLANDSE GEMEENTEN</t>
+  </si>
+  <si>
+    <t>BNP PARIBAS</t>
+  </si>
+  <si>
+    <t>BANK OF AMERICA</t>
+  </si>
+  <si>
+    <t>BANK OF SCOTLAND, AMSTERDAM</t>
+  </si>
+  <si>
+    <t>MUFG BANK</t>
+  </si>
+  <si>
+    <t>CITCO BANK</t>
+  </si>
+  <si>
+    <t>CITIBANK INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>COMMERZBANK</t>
+  </si>
+  <si>
+    <t>DEUTSCHE BANK (bij alle SEPA-transacties)</t>
+  </si>
+  <si>
+    <t>DEMIR-HALK BANK</t>
+  </si>
+  <si>
+    <t>DELTA LLOYD BANK</t>
+  </si>
+  <si>
+    <t>CREDIT EUROPE BANK</t>
+  </si>
+  <si>
+    <t>FGH BANK</t>
+  </si>
+  <si>
+    <t>DE NEDERLANDSCHE BANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THEODOOR GILISSEN </t>
+  </si>
+  <si>
+    <t>INSINGER DE BEAUFORT</t>
+  </si>
+  <si>
+    <t>YAPI KREDI BANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAS BANK </t>
+  </si>
+  <si>
+    <t>KBC BANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLOYDS TSB BANK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEASEPLAN CORPORATION </t>
+  </si>
+  <si>
+    <t>MIZUHO BANK EUROPE NV</t>
+  </si>
+  <si>
+    <t>NATIONALE-NEDERLANDEN BANK</t>
+  </si>
+  <si>
+    <t>NEDERLANDSE WATERSCHAPSBANK</t>
+  </si>
+  <si>
+    <t>CHINA CONSTRUCTION BANK, AMSTERDAM BRANCH</t>
+  </si>
+  <si>
+    <t>RABOBANK</t>
+  </si>
+  <si>
+    <t>TRIODOS BANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THE ECONOMY BANK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARANTIBANK INTERNATIONAL </t>
+  </si>
+  <si>
+    <t>MOYO</t>
+  </si>
+  <si>
+    <t>MOYONL21</t>
+  </si>
+  <si>
+    <t>MONEYOU</t>
+  </si>
+  <si>
+    <t>ADYB</t>
+  </si>
+  <si>
+    <t>ADYBNL2A</t>
+  </si>
+  <si>
+    <t>BNDA</t>
+  </si>
+  <si>
+    <t>BNDANL2A</t>
+  </si>
+  <si>
+    <t>Laatste update: 14-07-2017</t>
+  </si>
+  <si>
     <t>ANAANL21</t>
   </si>
   <si>
-    <t>ALLIANZ NEDERLAND ASSET MANAGEMENT</t>
-  </si>
-  <si>
-    <t>BKCH</t>
-  </si>
-  <si>
-    <t>BANK OF CHINA</t>
-  </si>
-  <si>
-    <t>BKCHNL2R</t>
-  </si>
-  <si>
-    <t>BMEU</t>
-  </si>
-  <si>
-    <t>BMEUNL21</t>
-  </si>
-  <si>
-    <t>BMCE EUROSERVICES</t>
-  </si>
-  <si>
-    <t>BINKNL21</t>
-  </si>
-  <si>
-    <t>BINK</t>
-  </si>
-  <si>
-    <t>BUNQ</t>
-  </si>
-  <si>
-    <t>BUNQNL2A</t>
-  </si>
-  <si>
-    <t>PCBC</t>
-  </si>
-  <si>
-    <t>PCBCNL2A</t>
-  </si>
-  <si>
-    <t>ABN AMRO BANK NV</t>
-  </si>
-  <si>
-    <t>AEGON BANK NV</t>
-  </si>
-  <si>
-    <t>ANADOLUBANK NEDERLAND NV</t>
-  </si>
-  <si>
-    <t>ACHMEA RETAIL BANK NV</t>
-  </si>
-  <si>
-    <t>ARGENTA SPAARBANK NV</t>
-  </si>
-  <si>
-    <t>AMSTERDAM TRADE BANK NV</t>
-  </si>
-  <si>
-    <t>BANQUE CHAABI DU MAROC</t>
-  </si>
-  <si>
-    <t>INTESA SANPAOLO SPA</t>
-  </si>
-  <si>
-    <t>BINCKBANK NV</t>
-  </si>
-  <si>
-    <t>BANK MENDES GANS NV</t>
-  </si>
-  <si>
-    <t>NV BANK NEDERLANDSE GEMEENTEN</t>
-  </si>
-  <si>
-    <t>BNP PARIBAS SA, NETHERLANDS BRANCH</t>
-  </si>
-  <si>
-    <t>BINCKBANK NV, PROF</t>
-  </si>
-  <si>
-    <t>BANK OF AMERICA NA</t>
-  </si>
-  <si>
-    <t>CREDIT EUROPE BANK NV</t>
-  </si>
-  <si>
-    <t>DE NEDERLANDSCHE BANK NV</t>
-  </si>
-  <si>
-    <t>BANK OF SCOTLAND PLC, AMSTERDAM BRANCH</t>
-  </si>
-  <si>
-    <t>BANK OF TOKYO-MITSUBISHI UFJ</t>
-  </si>
-  <si>
-    <t>CITCO BANK NEDERLAND</t>
-  </si>
-  <si>
-    <t>COMMERZBANK AG</t>
-  </si>
-  <si>
-    <t>DEUTSCHE BANK</t>
-  </si>
-  <si>
-    <t>DEMIR-HALK BANK (NEDERLAND) NV</t>
-  </si>
-  <si>
-    <t>DELTA LLOYD BANK NV</t>
-  </si>
-  <si>
-    <t>NIBC BANK NV</t>
-  </si>
-  <si>
-    <t>F.VAN LANSCHOT BANKIERS NV</t>
-  </si>
-  <si>
-    <t>THEODOOR GILISSEN NV</t>
-  </si>
-  <si>
-    <t>HSBC BANK PLC</t>
-  </si>
-  <si>
-    <t>ING BANK NV</t>
-  </si>
-  <si>
-    <t>ISBANK</t>
-  </si>
-  <si>
-    <t>INSINGER DE BEAUFORT NV</t>
-  </si>
-  <si>
-    <t>YAPI KREDI BANK NEDERLAND NV</t>
-  </si>
-  <si>
-    <t>KAS BANK NV</t>
-  </si>
-  <si>
-    <t>KOREA EXCHANGE BANK</t>
-  </si>
-  <si>
-    <t>KBC BANK NEDERLAND NV</t>
-  </si>
-  <si>
-    <t>LLOYDS TSB BANK PLC</t>
-  </si>
-  <si>
-    <t>LEASEPLAN CORPORATION NV</t>
-  </si>
-  <si>
-    <t>MIZUHO CORPORATE BANK NEDERLAND NV</t>
-  </si>
-  <si>
-    <t>NATIONALE-NEDERLANDEN BANK NV</t>
-  </si>
-  <si>
-    <t>NEDERLANDSE WATERSCHAPSBANK NV</t>
-  </si>
-  <si>
-    <t>CHINA CONSTRUCTION BANK SA, AMSTERDAM BRANCH</t>
-  </si>
-  <si>
-    <t>RABOBANK GROEP</t>
-  </si>
-  <si>
-    <t>ROYAL BANK OF SCOTLAND</t>
-  </si>
-  <si>
-    <t>SNS BANK NV</t>
-  </si>
-  <si>
-    <t>SOCIETE GENERALE</t>
-  </si>
-  <si>
-    <t>STAALBANKIERS NV</t>
-  </si>
-  <si>
-    <t>THE ECONOMY BANK NV</t>
-  </si>
-  <si>
-    <t>TRIODOS BANK NV</t>
-  </si>
-  <si>
-    <t>UBS BANK (NETHERLANDS) BV</t>
-  </si>
-  <si>
-    <t>GARANTIBANK INTERNATIONAL NV</t>
-  </si>
-  <si>
-    <t>VOLKSWAGEN BANK</t>
-  </si>
-  <si>
-    <t>Laatste update: 4 maart 2016</t>
+    <t>ABN AMRO (ex FORTIS)</t>
+  </si>
+  <si>
+    <t>ADYEN</t>
+  </si>
+  <si>
+    <t>BRAND NEW DAY BANK (EX ALIANZ ASSESMENT MANAGMENT)</t>
+  </si>
+  <si>
+    <t>BRAND NEW DAY BANK</t>
+  </si>
+  <si>
+    <t>NIBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAN LANSCHOT </t>
+  </si>
+  <si>
+    <t>SVENSKA HANDELSBANKEN</t>
+  </si>
+  <si>
+    <t>HSBC BANK</t>
+  </si>
+  <si>
+    <t>INDUSTRIAL &amp; COMMERCIAL BANK OF CHINA</t>
+  </si>
+  <si>
+    <t>ING</t>
+  </si>
+  <si>
+    <t>SNS</t>
+  </si>
+  <si>
+    <t>UBS EUROPE, NETHERLANDS BRANCH</t>
+  </si>
+  <si>
+    <t>SNS ( ex ZWITSERLEVENBANK)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -742,18 +766,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -763,6 +788,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -811,7 +839,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -846,7 +874,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1058,773 +1086,784 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="56.42578125" customWidth="1"/>
+    <col min="3" max="3" width="61.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="A1" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>187</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>136</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>158</v>
+        <v>50</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>145</v>
+        <v>51</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="4" t="s">
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="4" t="s">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="4" t="s">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="B40" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="B41" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="B45" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="B46" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="B47" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="C48" s="4" t="s">
-        <v>102</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>183</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>1</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>110</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>193</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>195</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>125</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BIC codes for all countries except LI. Updated sources
</commit_message>
<xml_diff>
--- a/data/nl.xlsx
+++ b/data/nl.xlsx
@@ -105,9 +105,6 @@
     <t>INGBNL2A</t>
   </si>
   <si>
-    <t>INSINL2A</t>
-  </si>
-  <si>
     <t>ISBKNL2A</t>
   </si>
   <si>
@@ -237,9 +234,6 @@
     <t>INGB</t>
   </si>
   <si>
-    <t>INSI</t>
-  </si>
-  <si>
     <t>ISBK</t>
   </si>
   <si>
@@ -384,9 +378,6 @@
     <t>BLG WONEN</t>
   </si>
   <si>
-    <t>DEUTNL2N</t>
-  </si>
-  <si>
     <t>ASN BANK</t>
   </si>
   <si>
@@ -525,12 +516,6 @@
     <t>DE NEDERLANDSCHE BANK</t>
   </si>
   <si>
-    <t xml:space="preserve">THEODOOR GILISSEN </t>
-  </si>
-  <si>
-    <t>INSINGER DE BEAUFORT</t>
-  </si>
-  <si>
     <t>YAPI KREDI BANK</t>
   </si>
   <si>
@@ -591,9 +576,6 @@
     <t>BNDANL2A</t>
   </si>
   <si>
-    <t>Laatste update: 14-07-2017</t>
-  </si>
-  <si>
     <t>ANAANL21</t>
   </si>
   <si>
@@ -634,6 +616,24 @@
   </si>
   <si>
     <t>SNS ( ex ZWITSERLEVENBANK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSINGERGILISSEN </t>
+  </si>
+  <si>
+    <t>DEUTNL2A</t>
+  </si>
+  <si>
+    <t>FRNX</t>
+  </si>
+  <si>
+    <t>FRNXNL2A</t>
+  </si>
+  <si>
+    <t>FRANX</t>
+  </si>
+  <si>
+    <t>Laatste update: 15-01-2018</t>
   </si>
 </sst>
 </file>
@@ -766,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -779,6 +779,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1088,8 +1089,8 @@
   </sheetPr>
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1101,14 +1102,14 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1119,561 +1120,561 @@
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>121</v>
+        <v>200</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="A38" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="C39" s="4" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>110</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>199</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>0</v>
@@ -1681,189 +1682,189 @@
     </row>
     <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>